<commit_message>
adding some flower parts
</commit_message>
<xml_diff>
--- a/docs/Error_summary.xlsx
+++ b/docs/Error_summary.xlsx
@@ -858,7 +858,7 @@
   <dimension ref="A1:O360"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A292" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C321" sqref="C321"/>
+      <selection activeCell="D303" sqref="D303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3630,7 +3630,7 @@
         <v>2676</v>
       </c>
       <c r="I123">
-        <f>E123-F123+H123-D123</f>
+        <f t="shared" ref="I123:I138" si="5">E123-F123+H123-D123</f>
         <v>0</v>
       </c>
       <c r="J123" s="2"/>
@@ -3659,7 +3659,7 @@
         <v>2902</v>
       </c>
       <c r="I124">
-        <f>E124-F124+H124-D124</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J124" s="2"/>
@@ -3688,7 +3688,7 @@
         <v>80024</v>
       </c>
       <c r="I125">
-        <f>E125-F125+H125-D125</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J125" s="2"/>
@@ -3711,7 +3711,7 @@
         <v>190594</v>
       </c>
       <c r="I126">
-        <f>E126-F126+H126-D126</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J126" s="2"/>
@@ -3740,7 +3740,7 @@
         <v>85696</v>
       </c>
       <c r="I127">
-        <f>E127-F127+H127-D127</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J127" s="2"/>
@@ -3763,7 +3763,7 @@
         <v>31930</v>
       </c>
       <c r="I128">
-        <f>E128-F128+H128-D128</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J128" s="2"/>
@@ -3792,7 +3792,7 @@
         <v>31672</v>
       </c>
       <c r="I129">
-        <f>E129-F129+H129-D129</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J129" s="2"/>
@@ -3822,7 +3822,7 @@
         <v>12</v>
       </c>
       <c r="I130">
-        <f>E130-F130+H130-D130</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J130" s="2"/>
@@ -3846,7 +3846,7 @@
         <v>176</v>
       </c>
       <c r="I131">
-        <f>E131-F131+H131-D131</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J131" s="2"/>
@@ -3871,7 +3871,7 @@
         <v>186</v>
       </c>
       <c r="I132">
-        <f>E132-F132+H132-D132</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J132" s="2"/>
@@ -3900,7 +3900,7 @@
         <v>6</v>
       </c>
       <c r="I133">
-        <f>E133-F133+H133-D133</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J133" s="2"/>
@@ -3923,7 +3923,7 @@
         <v>78</v>
       </c>
       <c r="I134">
-        <f>E134-F134+H134-D134</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J134" s="2"/>
@@ -3950,7 +3950,7 @@
         <v>232</v>
       </c>
       <c r="I135">
-        <f>E135-F135+H135-D135</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J135" s="2"/>
@@ -3979,7 +3979,7 @@
         <v>102</v>
       </c>
       <c r="I136">
-        <f>E136-F136+H136-D136</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J136" s="2"/>
@@ -4002,7 +4002,7 @@
         <v>130</v>
       </c>
       <c r="I137">
-        <f>E137-F137+H137-D137</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J137" s="2"/>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="F138" s="1"/>
       <c r="I138">
-        <f>E138-F138+H138-D138</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J138" s="2"/>
@@ -4109,7 +4109,7 @@
         <v>6</v>
       </c>
       <c r="I144">
-        <f>E144-F144+H144-D144</f>
+        <f t="shared" ref="I144:I153" si="6">E144-F144+H144-D144</f>
         <v>0</v>
       </c>
     </row>
@@ -4139,7 +4139,7 @@
         <v>13</v>
       </c>
       <c r="I145">
-        <f>E145-F145+H145-D145</f>
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
       <c r="J145" t="s">
@@ -4169,7 +4169,7 @@
         <v>65</v>
       </c>
       <c r="I146">
-        <f>E146-F146+H146-D146</f>
+        <f t="shared" si="6"/>
         <v>-5</v>
       </c>
       <c r="J146" t="s">
@@ -4205,7 +4205,7 @@
         <v>6</v>
       </c>
       <c r="I147">
-        <f>E147-F147+H147-D147</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
         <v>13</v>
       </c>
       <c r="I148">
-        <f>E148-F148+H148-D148</f>
+        <f t="shared" si="6"/>
         <v>-9</v>
       </c>
       <c r="J148" t="s">
@@ -4265,7 +4265,7 @@
         <v>73</v>
       </c>
       <c r="I149">
-        <f>E149-F149+H149-D149</f>
+        <f t="shared" si="6"/>
         <v>-9</v>
       </c>
       <c r="J149" t="s">
@@ -4292,7 +4292,7 @@
         <v>12</v>
       </c>
       <c r="I150">
-        <f>E150-F150+H150-D150</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4322,7 +4322,7 @@
         <v>12</v>
       </c>
       <c r="I151">
-        <f>E151-F151+H151-D151</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4346,7 +4346,7 @@
         <v>3</v>
       </c>
       <c r="I152">
-        <f>E152-F152+H152-D152</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4376,7 +4376,7 @@
         <v>50</v>
       </c>
       <c r="I153">
-        <f>E153-F153+H153-D153</f>
+        <f t="shared" si="6"/>
         <v>-4</v>
       </c>
       <c r="J153" t="s">
@@ -4470,7 +4470,7 @@
         <v>32</v>
       </c>
       <c r="I160">
-        <f t="shared" ref="I160:I172" si="5">E160-F160+H160-D160</f>
+        <f t="shared" ref="I160:I172" si="7">E160-F160+H160-D160</f>
         <v>0</v>
       </c>
       <c r="J160" s="2"/>
@@ -4500,7 +4500,7 @@
         <v>4</v>
       </c>
       <c r="I161">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J161" s="2"/>
@@ -4530,7 +4530,7 @@
         <v>74</v>
       </c>
       <c r="I162">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J162" s="2"/>
@@ -4554,7 +4554,7 @@
         <v>319</v>
       </c>
       <c r="I163">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J163" s="2"/>
@@ -4578,7 +4578,7 @@
         <v>4071</v>
       </c>
       <c r="I164">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J164" s="2"/>
@@ -4602,7 +4602,7 @@
         <v>2997</v>
       </c>
       <c r="I165">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J165" s="2"/>
@@ -4632,7 +4632,7 @@
         <v>195</v>
       </c>
       <c r="I166">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J166" s="2"/>
@@ -4662,7 +4662,7 @@
         <v>261</v>
       </c>
       <c r="I167">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J167" s="2"/>
@@ -4692,7 +4692,7 @@
         <v>47</v>
       </c>
       <c r="I168">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J168" s="2"/>
@@ -4719,7 +4719,7 @@
         <v>1617</v>
       </c>
       <c r="I169">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J169" s="2"/>
@@ -4749,7 +4749,7 @@
         <v>408</v>
       </c>
       <c r="I170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J170" s="2"/>
@@ -4773,7 +4773,7 @@
         <v>1323</v>
       </c>
       <c r="I171">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J171" s="2"/>
@@ -4800,7 +4800,7 @@
         <v>572</v>
       </c>
       <c r="I172">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J172" s="2"/>
@@ -4884,7 +4884,7 @@
         <v>1</v>
       </c>
       <c r="I178">
-        <f t="shared" ref="I178:I194" si="6">E178-F178+H178-D178</f>
+        <f t="shared" ref="I178:I194" si="8">E178-F178+H178-D178</f>
         <v>0</v>
       </c>
       <c r="J178" s="2"/>
@@ -4915,7 +4915,7 @@
       </c>
       <c r="H179" s="1"/>
       <c r="I179">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J179" s="2"/>
@@ -4945,7 +4945,7 @@
         <v>106</v>
       </c>
       <c r="I180">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J180" s="2"/>
@@ -4969,7 +4969,7 @@
         <v>1013</v>
       </c>
       <c r="I181">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J181" s="2"/>
@@ -4996,7 +4996,7 @@
         <v>330</v>
       </c>
       <c r="I182">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J182" s="2"/>
@@ -5026,7 +5026,7 @@
         <v>85</v>
       </c>
       <c r="I183">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J183" s="2"/>
@@ -5056,7 +5056,7 @@
         <v>172</v>
       </c>
       <c r="I184">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J184" s="2"/>
@@ -5089,7 +5089,7 @@
         <v>48</v>
       </c>
       <c r="I185">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J185" s="2"/>
@@ -5122,7 +5122,7 @@
         <v>282</v>
       </c>
       <c r="I186">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J186" s="2"/>
@@ -5152,7 +5152,7 @@
         <v>21</v>
       </c>
       <c r="I187">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J187" s="2"/>
@@ -5182,7 +5182,7 @@
         <v>35</v>
       </c>
       <c r="I188">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J188" s="2"/>
@@ -5212,7 +5212,7 @@
         <v>6</v>
       </c>
       <c r="I189">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J189" s="2"/>
@@ -5242,7 +5242,7 @@
         <v>1</v>
       </c>
       <c r="I190">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J190" s="2"/>
@@ -5272,7 +5272,7 @@
         <v>2</v>
       </c>
       <c r="I191">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J191" s="2"/>
@@ -5302,7 +5302,7 @@
         <v>1</v>
       </c>
       <c r="I192">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J192" s="2"/>
@@ -5326,7 +5326,7 @@
         <v>133</v>
       </c>
       <c r="I193">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J193" s="2"/>
@@ -5350,7 +5350,7 @@
         <v>133</v>
       </c>
       <c r="I194">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J194" s="2"/>
@@ -5453,7 +5453,7 @@
         <v>17</v>
       </c>
       <c r="I203">
-        <f t="shared" ref="I203:I223" si="7">E203-F203+H203-D203</f>
+        <f t="shared" ref="I203:I223" si="9">E203-F203+H203-D203</f>
         <v>0</v>
       </c>
       <c r="J203" s="2"/>
@@ -5476,7 +5476,7 @@
         <v>14</v>
       </c>
       <c r="I204">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J204" s="2"/>
@@ -5499,7 +5499,7 @@
         <v>11</v>
       </c>
       <c r="I205">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J205" s="2"/>
@@ -5522,7 +5522,7 @@
         <v>5</v>
       </c>
       <c r="I206">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J206" s="2"/>
@@ -5545,7 +5545,7 @@
         <v>1</v>
       </c>
       <c r="I207">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J207" s="2"/>
@@ -5568,7 +5568,7 @@
         <v>11</v>
       </c>
       <c r="I208">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J208" s="2"/>
@@ -5591,7 +5591,7 @@
         <v>11</v>
       </c>
       <c r="I209">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J209" s="2"/>
@@ -5614,7 +5614,7 @@
         <v>9</v>
       </c>
       <c r="I210">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J210" s="2"/>
@@ -5637,7 +5637,7 @@
         <v>12</v>
       </c>
       <c r="I211">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J211" s="2"/>
@@ -5660,7 +5660,7 @@
         <v>5</v>
       </c>
       <c r="I212">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J212" s="2"/>
@@ -5689,7 +5689,7 @@
         <v>11</v>
       </c>
       <c r="I213">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J213" s="2"/>
@@ -5717,7 +5717,7 @@
         <v>9</v>
       </c>
       <c r="I214">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J214" s="2"/>
@@ -5740,7 +5740,7 @@
         <v>916</v>
       </c>
       <c r="I215">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J215" s="2"/>
@@ -5763,7 +5763,7 @@
         <v>916</v>
       </c>
       <c r="I216">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J216" s="2"/>
@@ -5792,7 +5792,7 @@
         <v>74</v>
       </c>
       <c r="I217">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J217" s="2"/>
@@ -5821,7 +5821,7 @@
         <v>16</v>
       </c>
       <c r="I218">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J218" s="2"/>
@@ -5844,7 +5844,7 @@
         <v>660</v>
       </c>
       <c r="I219">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J219" s="2"/>
@@ -5867,7 +5867,7 @@
         <v>140</v>
       </c>
       <c r="I220">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J220" s="2"/>
@@ -5896,7 +5896,7 @@
         <v>17</v>
       </c>
       <c r="I221">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J221" s="2"/>
@@ -5919,7 +5919,7 @@
         <v>409</v>
       </c>
       <c r="I222">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J222" s="2"/>
@@ -5942,7 +5942,7 @@
         <v>260</v>
       </c>
       <c r="I223">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J223" s="2"/>
@@ -6023,7 +6023,7 @@
         <v>312</v>
       </c>
       <c r="I229">
-        <f t="shared" ref="I229:I245" si="8">E229-F229+H229-D229</f>
+        <f t="shared" ref="I229:I245" si="10">E229-F229+H229-D229</f>
         <v>0</v>
       </c>
       <c r="J229" s="2"/>
@@ -6049,7 +6049,7 @@
       </c>
       <c r="G230" s="1"/>
       <c r="I230">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J230" s="2"/>
@@ -6073,7 +6073,7 @@
         <v>974</v>
       </c>
       <c r="I231">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K231" s="2"/>
@@ -6096,7 +6096,7 @@
         <v>72</v>
       </c>
       <c r="I232">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J232" s="2"/>
@@ -6120,7 +6120,7 @@
         <v>4748</v>
       </c>
       <c r="I233">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J233" s="2"/>
@@ -6147,7 +6147,7 @@
         <v>470</v>
       </c>
       <c r="I234">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J234" s="2"/>
@@ -6171,7 +6171,7 @@
         <v>5218</v>
       </c>
       <c r="I235">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K235" s="2"/>
@@ -6194,7 +6194,7 @@
         <v>5218</v>
       </c>
       <c r="I236">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J236" s="2"/>
@@ -6224,7 +6224,7 @@
         <v>812</v>
       </c>
       <c r="I237">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K237" s="2"/>
@@ -6253,7 +6253,7 @@
         <v>3410</v>
       </c>
       <c r="I238">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J238" s="2"/>
@@ -6283,7 +6283,7 @@
         <v>401</v>
       </c>
       <c r="I239">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K239" s="2"/>
@@ -6312,7 +6312,7 @@
         <v>167</v>
       </c>
       <c r="I240">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K240" s="2"/>
@@ -6341,7 +6341,7 @@
         <v>60</v>
       </c>
       <c r="I241">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K241" s="2"/>
@@ -6364,7 +6364,7 @@
         <v>122</v>
       </c>
       <c r="I242">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K242" s="2"/>
@@ -6387,7 +6387,7 @@
         <v>72</v>
       </c>
       <c r="I243">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K243" s="2"/>
@@ -6410,7 +6410,7 @@
         <v>174</v>
       </c>
       <c r="I244">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K244" s="2"/>
@@ -6433,7 +6433,7 @@
         <v>584</v>
       </c>
       <c r="I245">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K245" s="2"/>
@@ -6549,7 +6549,7 @@
         <v>4</v>
       </c>
       <c r="I253">
-        <f t="shared" ref="I253:I264" si="9">E253-F253+H253-D253</f>
+        <f t="shared" ref="I253:I264" si="11">E253-F253+H253-D253</f>
         <v>0</v>
       </c>
     </row>
@@ -6574,7 +6574,7 @@
         <v>1</v>
       </c>
       <c r="I254">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6598,7 +6598,7 @@
         <v>1</v>
       </c>
       <c r="I255">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6625,7 +6625,7 @@
         <v>23</v>
       </c>
       <c r="I256">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6649,7 +6649,7 @@
         <v>5</v>
       </c>
       <c r="I257">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6673,7 +6673,7 @@
         <v>5</v>
       </c>
       <c r="I258">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6703,7 +6703,7 @@
         <v>5</v>
       </c>
       <c r="I259">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6731,7 +6731,7 @@
       </c>
       <c r="H260" s="1"/>
       <c r="I260">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6759,7 +6759,7 @@
       </c>
       <c r="H261" s="1"/>
       <c r="I261">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6781,7 +6781,7 @@
       </c>
       <c r="H262" s="1"/>
       <c r="I262">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6802,7 +6802,7 @@
         <v>253</v>
       </c>
       <c r="I263">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6823,7 +6823,7 @@
         <v>253</v>
       </c>
       <c r="I264">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6910,7 +6910,7 @@
         <v>18</v>
       </c>
       <c r="I271">
-        <f t="shared" ref="I271:I282" si="10">E271-F271+H271-D271</f>
+        <f t="shared" ref="I271:I282" si="12">E271-F271+H271-D271</f>
         <v>0</v>
       </c>
     </row>
@@ -6931,7 +6931,7 @@
         <v>834</v>
       </c>
       <c r="I272">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -6952,7 +6952,7 @@
         <v>3756</v>
       </c>
       <c r="I273">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -6973,7 +6973,7 @@
         <v>3756</v>
       </c>
       <c r="I274">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -6994,7 +6994,7 @@
         <v>3756</v>
       </c>
       <c r="I275">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7021,7 +7021,7 @@
         <v>6</v>
       </c>
       <c r="I276">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7042,7 +7042,7 @@
         <v>32</v>
       </c>
       <c r="I277">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7072,7 +7072,7 @@
         <v>140</v>
       </c>
       <c r="I278">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J278" t="s">
@@ -7102,7 +7102,7 @@
         <v>429</v>
       </c>
       <c r="I279">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7123,7 +7123,7 @@
         <v>201</v>
       </c>
       <c r="I280">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7144,7 +7144,7 @@
         <v>292</v>
       </c>
       <c r="I281">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7165,7 +7165,7 @@
         <v>940</v>
       </c>
       <c r="I282">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7242,7 +7242,7 @@
         <v>236</v>
       </c>
       <c r="F289">
-        <f t="shared" ref="F289:F299" si="11">D289-E289</f>
+        <f t="shared" ref="F289:F299" si="13">D289-E289</f>
         <v>-50</v>
       </c>
       <c r="I289" s="4"/>
@@ -7261,7 +7261,7 @@
         <v>168</v>
       </c>
       <c r="F290">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-32</v>
       </c>
       <c r="I290" s="4"/>
@@ -7280,7 +7280,7 @@
         <v>264</v>
       </c>
       <c r="F291">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-26</v>
       </c>
       <c r="I291" s="4"/>
@@ -7299,7 +7299,7 @@
         <v>116</v>
       </c>
       <c r="F292">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-10</v>
       </c>
       <c r="H292">
@@ -7322,7 +7322,7 @@
         <v>46</v>
       </c>
       <c r="F293">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-6</v>
       </c>
       <c r="I293" s="4"/>
@@ -7341,7 +7341,7 @@
         <v>300</v>
       </c>
       <c r="F294">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-4</v>
       </c>
       <c r="I294" s="4"/>
@@ -7360,7 +7360,7 @@
         <v>170</v>
       </c>
       <c r="F295">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-4</v>
       </c>
       <c r="I295" s="4"/>
@@ -7379,7 +7379,7 @@
         <v>96</v>
       </c>
       <c r="F296">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-2</v>
       </c>
       <c r="I296" s="4"/>
@@ -7398,7 +7398,7 @@
         <v>188</v>
       </c>
       <c r="F297">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-2</v>
       </c>
       <c r="I297" s="4"/>
@@ -7417,7 +7417,7 @@
         <v>32</v>
       </c>
       <c r="F298">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-2</v>
       </c>
       <c r="I298" s="4"/>
@@ -7436,7 +7436,7 @@
         <v>88</v>
       </c>
       <c r="F299">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-2</v>
       </c>
       <c r="I299" s="4"/>
@@ -7480,14 +7480,14 @@
         <v>770</v>
       </c>
       <c r="F303" s="1">
-        <v>560</v>
+        <v>572</v>
       </c>
       <c r="G303" s="1">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="I303">
-        <f t="shared" ref="I303:I320" si="12">E303-F303+H303-D303</f>
-        <v>14</v>
+        <f t="shared" ref="I303:I320" si="14">E303-F303+H303-D303</f>
+        <v>2</v>
       </c>
     </row>
     <row r="304" spans="2:12" x14ac:dyDescent="0.25">
@@ -7504,14 +7504,14 @@
         <v>2074</v>
       </c>
       <c r="F304" s="1">
-        <v>958</v>
+        <v>1056</v>
       </c>
       <c r="G304" s="1">
-        <v>1104</v>
+        <v>1010</v>
       </c>
       <c r="I304">
-        <f t="shared" si="12"/>
-        <v>106</v>
+        <f t="shared" si="14"/>
+        <v>8</v>
       </c>
       <c r="J304" s="2"/>
       <c r="K304" s="1"/>
@@ -7536,7 +7536,7 @@
         <v>102</v>
       </c>
       <c r="I305">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J305" s="2"/>
@@ -7556,17 +7556,17 @@
         <v>2784</v>
       </c>
       <c r="F306" s="1">
-        <v>2056</v>
+        <v>1858</v>
       </c>
       <c r="G306" s="1">
-        <v>708</v>
+        <v>906</v>
       </c>
       <c r="H306">
         <v>40</v>
       </c>
       <c r="I306">
-        <f t="shared" si="12"/>
-        <v>-198</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="J306" s="2"/>
       <c r="K306" s="1"/>
@@ -7582,10 +7582,10 @@
         <v>-66</v>
       </c>
       <c r="G307" s="1">
-        <v>-74</v>
+        <v>-66</v>
       </c>
       <c r="I307">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>66</v>
       </c>
       <c r="J307" s="2"/>
@@ -7605,7 +7605,7 @@
         <v>4048</v>
       </c>
       <c r="I308">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J308" s="2"/>
@@ -7622,17 +7622,17 @@
         <v>3120</v>
       </c>
       <c r="E309" s="1">
-        <v>3624</v>
+        <v>3734</v>
       </c>
       <c r="F309" s="1">
-        <v>546</v>
+        <v>554</v>
       </c>
       <c r="G309" s="1">
-        <v>3000</v>
+        <v>3096</v>
       </c>
       <c r="I309">
-        <f t="shared" si="12"/>
-        <v>-42</v>
+        <f t="shared" si="14"/>
+        <v>60</v>
       </c>
       <c r="J309" s="2"/>
       <c r="K309" s="1"/>
@@ -7651,14 +7651,14 @@
         <v>556</v>
       </c>
       <c r="F310" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G310" s="1">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="I310">
-        <f t="shared" si="12"/>
-        <v>-6</v>
+        <f t="shared" si="14"/>
+        <v>-4</v>
       </c>
       <c r="J310" s="2"/>
       <c r="K310" s="1"/>
@@ -7674,17 +7674,17 @@
         <v>40</v>
       </c>
       <c r="E311" s="1">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F311" s="1">
         <v>96</v>
       </c>
       <c r="G311" s="1">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I311">
-        <f t="shared" si="12"/>
-        <v>-54</v>
+        <f t="shared" si="14"/>
+        <v>-58</v>
       </c>
       <c r="J311" s="2"/>
       <c r="K311" s="1"/>
@@ -7700,17 +7700,17 @@
         <v>2</v>
       </c>
       <c r="E312" s="1">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F312" s="1">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G312" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I312">
-        <f t="shared" si="12"/>
-        <v>6</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="J312" s="2"/>
       <c r="K312" s="1"/>
@@ -7725,9 +7725,19 @@
       <c r="D313" s="1">
         <v>2</v>
       </c>
-      <c r="E313" s="1"/>
-      <c r="F313" s="1"/>
-      <c r="G313" s="1"/>
+      <c r="E313" s="1">
+        <v>6</v>
+      </c>
+      <c r="F313" s="1">
+        <v>4</v>
+      </c>
+      <c r="G313" s="1">
+        <v>2</v>
+      </c>
+      <c r="I313">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="J313" s="2"/>
       <c r="K313" s="1"/>
     </row>
@@ -7742,17 +7752,17 @@
         <v>34</v>
       </c>
       <c r="E314" s="1">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F314" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G314" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I314">
-        <f t="shared" si="12"/>
-        <v>-14</v>
+        <f t="shared" si="14"/>
+        <v>-4</v>
       </c>
       <c r="J314" s="2"/>
       <c r="K314" s="1"/>
@@ -7777,7 +7787,7 @@
         <v>18</v>
       </c>
       <c r="I315">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J315" s="2"/>
@@ -7797,7 +7807,7 @@
         <v>130</v>
       </c>
       <c r="I316">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J316" s="2"/>
@@ -7817,7 +7827,7 @@
         <v>78</v>
       </c>
       <c r="I317">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-58</v>
       </c>
       <c r="J317" s="2"/>
@@ -7834,11 +7844,11 @@
         <v>69</v>
       </c>
       <c r="E318" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I318">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="J318" s="2"/>
       <c r="K318" s="1"/>
@@ -7854,11 +7864,11 @@
         <v>25</v>
       </c>
       <c r="E319" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I319">
-        <f t="shared" si="12"/>
-        <v>-3</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="J319" s="2"/>
       <c r="K319" s="1"/>
@@ -7874,11 +7884,11 @@
         <v>94</v>
       </c>
       <c r="E320" s="1">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I320">
-        <f t="shared" si="12"/>
-        <v>-2</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="J320" s="2"/>
       <c r="K320" s="1"/>
@@ -7926,6 +7936,9 @@
       <c r="D325" s="1">
         <v>4048</v>
       </c>
+      <c r="E325">
+        <v>3774</v>
+      </c>
     </row>
     <row r="326" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C326" s="2"/>
@@ -8035,8 +8048,8 @@
       <c r="E360" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="J306:K324">
-    <sortCondition ref="J306:J324"/>
+  <sortState ref="J306:K316">
+    <sortCondition ref="J306:J316"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>